<commit_message>
Fixed bugs with excel print
</commit_message>
<xml_diff>
--- a/excels/Дорофеев Андрей Сергеевич.xlsx
+++ b/excels/Дорофеев Андрей Сергеевич.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="17">
   <si>
     <t>Здравствуйте, Дорофеев Андрей Сергеевич</t>
   </si>
@@ -44,16 +44,28 @@
     <t>Гамф</t>
   </si>
   <si>
+    <t>Вторник</t>
+  </si>
+  <si>
+    <t>11:45:00</t>
+  </si>
+  <si>
+    <t>Базы данных - практика</t>
+  </si>
+  <si>
+    <t>В100</t>
+  </si>
+  <si>
     <t>Среда</t>
   </si>
   <si>
-    <t>11:45:00</t>
-  </si>
-  <si>
-    <t>Базы данных - практика</t>
-  </si>
-  <si>
-    <t>В100</t>
+    <t>Пятница</t>
+  </si>
+  <si>
+    <t>13:45:00</t>
+  </si>
+  <si>
+    <t>В101</t>
   </si>
 </sst>
 </file>
@@ -393,7 +405,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,6 +460,34 @@
         <v>12</v>
       </c>
     </row>
+    <row r="7" spans="1:5">
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>